<commit_message>
update1 after review 1
</commit_message>
<xml_diff>
--- a/ppt and references/references.xlsx
+++ b/ppt and references/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mini ke saath project\review 1\ppt and references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F3158E-8993-4014-BD80-525BEBC23A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ABB509-4460-49B9-8784-D42D3D813486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +386,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -416,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,6 +459,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -845,7 +854,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="4" t="s">

</xml_diff>